<commit_message>
Update Mexican_EPUs.xlsx - 2026-01-05
</commit_message>
<xml_diff>
--- a/Mexican_EPUs.xlsx
+++ b/Mexican_EPUs.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Generated: 2026-01-05 13:52:20</t>
+          <t>Generated: 2026-01-05 14:36</t>
         </is>
       </c>
     </row>
@@ -465,86 +465,90 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>This workbook contains EPU indices for Mexico from multiple sources.</t>
+          <t>Methodology</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>This workbook contains EPU indices for Mexico from multiple sources:</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Data Sources:</t>
+          <t>• Monthly: Official EPU index from PolicyUncertainty.com (Baker, Bloom &amp; Davis)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Monthly (historical): PolicyUncertainty.com (1985-2025)</t>
+          <t>• Daily/Weekly: News-based keyword analysis of Mexican news articles</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  - Daily/Weekly/Monthly (recent): News-based keyword analysis</t>
-        </is>
-      </c>
+      <c r="A9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Data Coverage</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sheets:</t>
+          <t>• Monthly Range: 1985-2025 (491 observations)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Monthly: Historical EPU index (1985-present) from PolicyUncertainty.com</t>
+          <t>• Daily Range: 2025-02-01 to 2026-01-04</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Daily: Recent daily EPU from news analysis</t>
+          <t>• Categories: Economic policy uncertainty across fiscal, monetary, trade, regulatory domains</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  - Weekly: Recent weekly EPU from news analysis</t>
-        </is>
-      </c>
+      <c r="A14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Sheets</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Monthly sheet uses the official EPU methodology from:</t>
+          <t>• Monthly: Historical EPU index from PolicyUncertainty.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Baker, Bloom &amp; Davis - 'Measuring Economic Policy Uncertainty'</t>
+          <t>• Daily: Recent daily EPU from Mexican news analysis</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">  www.PolicyUncertainty.com</t>
+          <t>• Weekly: Recent weekly EPU from Mexican news analysis</t>
         </is>
       </c>
     </row>
@@ -554,24 +558,118 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Daily/Weekly sheets derived from Mexican news article classification.</t>
+          <t>Legal Disclaimer</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>This data is provided for informational purposes only. The author and data provider:</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Source: Monitoring Monetary Policy in Mexico project</t>
+          <t>• Make no warranties or guarantees about accuracy or completeness</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>URL: https://github.com/adentler1/MonitoringMexico</t>
+          <t>• Accept no liability for decisions made based on this data</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>• Recommend verifying with official sources for critical decisions</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>• Disclaim responsibility for any financial losses from use of this data</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>License</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CC0-1.0 (Creative Commons Zero)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>This dataset is dedicated to the public domain. You are free to:</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>• Copy, modify, and distribute the data</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>• Use for commercial or non-commercial purposes</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>• No attribution required (but appreciated)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>References</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>• Baker, Bloom &amp; Davis - "Measuring Economic Policy Uncertainty"</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>• www.PolicyUncertainty.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>• https://github.com/adentler1/MonitoringMexico</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Mexican_EPUs.xlsx - 2026-01-09
</commit_message>
<xml_diff>
--- a/Mexican_EPUs.xlsx
+++ b/Mexican_EPUs.xlsx
@@ -456,7 +456,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Generated: 2026-01-08 23:30</t>
+          <t>Generated: 2026-01-09 11:25</t>
         </is>
       </c>
     </row>
@@ -580,14 +580,14 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>• Weekly: 2025-01-28 to 2025-12-30 (45 periods, 9,607 total articles)</t>
+          <t>• Weekly: 2025-01-28 to 2026-01-06 (46 periods, 9,635 total articles)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>• Daily: 2025-02-01 to 2026-01-05 (307 periods, 9,607 total articles)</t>
+          <t>• Daily: 2025-02-01 to 2026-01-06 (308 periods, 9,635 total articles)</t>
         </is>
       </c>
     </row>
@@ -21933,7 +21933,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24474,52 +24474,107 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C46" t="n">
-        <v>16.9</v>
+        <v>15.94</v>
       </c>
       <c r="D46" t="n">
-        <v>2.82</v>
+        <v>2.9</v>
       </c>
       <c r="E46" t="n">
-        <v>9.859999999999999</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="F46" t="n">
-        <v>7.04</v>
+        <v>5.8</v>
       </c>
       <c r="G46" t="n">
-        <v>5.63</v>
+        <v>4.35</v>
       </c>
       <c r="H46" t="n">
-        <v>4.23</v>
+        <v>4.35</v>
       </c>
       <c r="I46" t="n">
-        <v>15.49</v>
+        <v>14.49</v>
       </c>
       <c r="J46" t="n">
-        <v>1.41</v>
+        <v>1.45</v>
       </c>
       <c r="K46" t="n">
         <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>4.23</v>
+        <v>4.35</v>
       </c>
       <c r="M46" t="n">
-        <v>22.54</v>
+        <v>21.74</v>
       </c>
       <c r="N46" t="n">
-        <v>18.31</v>
+        <v>17.39</v>
       </c>
       <c r="O46" t="n">
-        <v>9.859999999999999</v>
+        <v>10.14</v>
       </c>
       <c r="P46" t="n">
-        <v>7.04</v>
+        <v>7.25</v>
       </c>
       <c r="Q46" t="n">
-        <v>7.04</v>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>30</v>
+      </c>
+      <c r="C47" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>10</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="M47" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="N47" t="n">
+        <v>16.67</v>
+      </c>
+      <c r="O47" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="P47" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>6.67</v>
       </c>
     </row>
   </sheetData>
@@ -24533,7 +24588,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q308"/>
+  <dimension ref="A1:Q309"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41264,28 +41319,28 @@
         </is>
       </c>
       <c r="B304" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C304" t="n">
         <v>25</v>
       </c>
       <c r="D304" t="n">
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="E304" t="n">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="F304" t="n">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="G304" t="n">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="H304" t="n">
         <v>0</v>
       </c>
       <c r="I304" t="n">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="J304" t="n">
         <v>0</v>
@@ -41303,13 +41358,13 @@
         <v>25</v>
       </c>
       <c r="O304" t="n">
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="P304" t="n">
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="Q304" t="n">
-        <v>12.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="305">
@@ -41484,28 +41539,28 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C308" t="n">
-        <v>11.11</v>
+        <v>10.53</v>
       </c>
       <c r="D308" t="n">
         <v>0</v>
       </c>
       <c r="E308" t="n">
-        <v>8.33</v>
+        <v>7.89</v>
       </c>
       <c r="F308" t="n">
-        <v>2.78</v>
+        <v>2.63</v>
       </c>
       <c r="G308" t="n">
-        <v>5.56</v>
+        <v>5.26</v>
       </c>
       <c r="H308" t="n">
-        <v>5.56</v>
+        <v>5.26</v>
       </c>
       <c r="I308" t="n">
-        <v>8.33</v>
+        <v>7.89</v>
       </c>
       <c r="J308" t="n">
         <v>0</v>
@@ -41514,22 +41569,77 @@
         <v>0</v>
       </c>
       <c r="L308" t="n">
-        <v>2.78</v>
+        <v>2.63</v>
       </c>
       <c r="M308" t="n">
+        <v>15.79</v>
+      </c>
+      <c r="N308" t="n">
+        <v>10.53</v>
+      </c>
+      <c r="O308" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="P308" t="n">
+        <v>7.89</v>
+      </c>
+      <c r="Q308" t="n">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2026-01-06</t>
+        </is>
+      </c>
+      <c r="B309" t="n">
+        <v>30</v>
+      </c>
+      <c r="C309" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="D309" t="n">
+        <v>0</v>
+      </c>
+      <c r="E309" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="F309" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="G309" t="n">
+        <v>0</v>
+      </c>
+      <c r="H309" t="n">
+        <v>0</v>
+      </c>
+      <c r="I309" t="n">
+        <v>10</v>
+      </c>
+      <c r="J309" t="n">
+        <v>0</v>
+      </c>
+      <c r="K309" t="n">
+        <v>0</v>
+      </c>
+      <c r="L309" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="M309" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="N309" t="n">
         <v>16.67</v>
       </c>
-      <c r="N308" t="n">
-        <v>11.11</v>
-      </c>
-      <c r="O308" t="n">
-        <v>5.56</v>
-      </c>
-      <c r="P308" t="n">
-        <v>8.33</v>
-      </c>
-      <c r="Q308" t="n">
-        <v>2.78</v>
+      <c r="O309" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="P309" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="Q309" t="n">
+        <v>6.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>